<commit_message>
2da ppt+ video tests+ scripts tests
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Pruebas/Casos de Prueba.xls.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Pruebas/Casos de Prueba.xls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Documentos\CAPSTONE_002D\Fase 2\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Documentos\CAPSTONE_002D\Fase 2\Evidencias Proyecto\Evidencias de documentación\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F34A11-2D9A-4CB4-9D81-7D7DBD52129D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB758416-7AAF-4C9D-8533-C69CBF12A927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>Elaborado por: www.pmoinformatica.com</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Usuario registrado exitosamente, confirmación en pantalla, datos guardados en BD.</t>
   </si>
   <si>
-    <t>Navegador Chrome 128+, conexión estable, BD SQLite.</t>
-  </si>
-  <si>
     <t>Validar formato de RUT y correo.</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>Validación de formulario</t>
-  </si>
-  <si>
-    <t>Email: "prueba@".</t>
   </si>
   <si>
     <t>Mensaje de error “Correo inválido”.</t>
@@ -231,9 +225,6 @@
     <t>Acceso concedido al dashboard de usuario.</t>
   </si>
   <si>
-    <t>Navegadores soportados, BD con usuarios creados.</t>
-  </si>
-  <si>
     <t>Sesión activa de usuario.</t>
   </si>
   <si>
@@ -264,19 +255,10 @@
     <t>Emisión de certificado en PDF</t>
   </si>
   <si>
-    <t>Validar que un vecino pueda generar certificado digital.</t>
-  </si>
-  <si>
     <t>Certificados</t>
   </si>
   <si>
     <t>Emisión de Certificados</t>
-  </si>
-  <si>
-    <t>Botón "Generar certificado".</t>
-  </si>
-  <si>
-    <t>Certificado PDF descargado con datos correctos.</t>
   </si>
   <si>
     <t>BD con datos del vecino, librería de PDF.</t>
@@ -304,9 +286,6 @@
   </si>
   <si>
     <t>Confirmación de postulación exitosa.</t>
-  </si>
-  <si>
-    <t>Navegador Chrome/Firefox.</t>
   </si>
   <si>
     <t>Validar formato de archivos adjuntos.</t>
@@ -351,12 +330,6 @@
     <t>Validación de reserva</t>
   </si>
   <si>
-    <t>Selección misma sala y horario ya reservado.</t>
-  </si>
-  <si>
-    <t>Mensaje de error “Horario no disponible”.</t>
-  </si>
-  <si>
     <t>Igual que TC-007.</t>
   </si>
   <si>
@@ -369,16 +342,10 @@
     <t>Notificación vía Email</t>
   </si>
   <si>
-    <t>Validar envío de correo tras reserva confirmada.</t>
-  </si>
-  <si>
     <t>Notificaciones</t>
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Confirmación de reserva.</t>
   </si>
   <si>
     <t>Email recibido en bandeja del usuario.</t>
@@ -387,16 +354,10 @@
     <t>Servidor n8n conectado a SMTP.</t>
   </si>
   <si>
-    <t>Validar spam.</t>
-  </si>
-  <si>
     <t>TC-010</t>
   </si>
   <si>
     <t>Notificación vía WhatsApp</t>
-  </si>
-  <si>
-    <t>Validar que tras reserva confirmada llegue mensaje por WhatsApp.</t>
   </si>
   <si>
     <t>WhatsApp</t>
@@ -406,9 +367,6 @@
   </si>
   <si>
     <t>n8n integrado con API WhatsApp.</t>
-  </si>
-  <si>
-    <t>Teléfono válido y registrado.</t>
   </si>
   <si>
     <t>TC-011</t>
@@ -432,9 +390,6 @@
     <t>Acceso denegado.</t>
   </si>
   <si>
-    <t>Django Roles.</t>
-  </si>
-  <si>
     <t>TC-012</t>
   </si>
   <si>
@@ -450,24 +405,71 @@
     <t>Acceso concedido al panel admin.</t>
   </si>
   <si>
-    <t>Django Admin.</t>
-  </si>
-  <si>
     <t>Casos de Pruebas de Software</t>
   </si>
   <si>
     <t>Proyecto: Junta360 Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar envío de avisos </t>
+  </si>
+  <si>
+    <t>Avisos</t>
+  </si>
+  <si>
+    <t>Validar que un vecino pueda solicitar certificado digital.</t>
+  </si>
+  <si>
+    <t>Botón "Enviar Solicitud".</t>
+  </si>
+  <si>
+    <t>Se agrega a la lista de solicitudes previas esperando la resolucion.</t>
+  </si>
+  <si>
+    <t>View Django Roles.</t>
+  </si>
+  <si>
+    <t>Navegador que permita Selenium.</t>
+  </si>
+  <si>
+    <t>Intentar reservar una reserva tomada.</t>
+  </si>
+  <si>
+    <t>No poder hacer ninguna accion.</t>
+  </si>
+  <si>
+    <t>Reservas creadas.</t>
+  </si>
+  <si>
+    <t>Log desde Cuenta Admin</t>
+  </si>
+  <si>
+    <t>Email: "prueba".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,35 +603,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,7 +856,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -873,7 +881,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -931,7 +939,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1100,26 +1108,26 @@
       <c r="H7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1135,13 +1143,13 @@
     </row>
     <row r="8" spans="1:26" ht="30" customHeight="1">
       <c r="A8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="10">
         <v>45930</v>
@@ -1150,34 +1158,34 @@
         <v>39</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>55</v>
+      <c r="L8" s="9" t="s">
+        <v>45</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1193,49 +1201,49 @@
     </row>
     <row r="9" spans="1:26" ht="30">
       <c r="A9" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" s="10">
         <v>45930</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="I9" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="K9" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1251,49 +1259,49 @@
     </row>
     <row r="10" spans="1:26" ht="30">
       <c r="A10" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="10">
         <v>45930</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1309,49 +1317,49 @@
     </row>
     <row r="11" spans="1:26" ht="45">
       <c r="A11" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>75</v>
+      <c r="C11" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="D11" s="10">
         <v>45930</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>78</v>
+      <c r="G11" s="12" t="s">
+        <v>127</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>79</v>
+      <c r="H11" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1367,49 +1375,49 @@
     </row>
     <row r="12" spans="1:26" ht="45">
       <c r="A12" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D12" s="10">
         <v>45930</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>89</v>
+      <c r="I12" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1425,49 +1433,49 @@
     </row>
     <row r="13" spans="1:26" ht="30">
       <c r="A13" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D13" s="10">
         <v>45930</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1483,49 +1491,49 @@
     </row>
     <row r="14" spans="1:26" ht="45">
       <c r="A14" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D14" s="10">
         <v>45930</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>104</v>
+      <c r="G14" s="15" t="s">
+        <v>131</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>105</v>
+      <c r="H14" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="L14" s="9" t="s">
+      <c r="M14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1541,49 +1549,49 @@
     </row>
     <row r="15" spans="1:26" ht="30">
       <c r="A15" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>110</v>
+      <c r="C15" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="D15" s="10">
         <v>45930</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>113</v>
+      <c r="G15" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>116</v>
+      <c r="J15" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="L15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -1599,49 +1607,49 @@
     </row>
     <row r="16" spans="1:26" ht="105" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>119</v>
+      <c r="C16" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="D16" s="10">
         <v>45930</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>113</v>
+      <c r="G16" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>123</v>
+      <c r="J16" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="L16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1657,49 +1665,49 @@
     </row>
     <row r="17" spans="1:26" ht="45">
       <c r="A17" s="9" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>125</v>
+      <c r="B17" s="15" t="s">
+        <v>111</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D17" s="10">
         <v>45930</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>130</v>
+      <c r="J17" s="9" t="s">
+        <v>44</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>131</v>
+      <c r="K17" s="9" t="s">
+        <v>69</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="L17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L17" s="9" t="s">
+      <c r="M17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M17" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -1713,51 +1721,51 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="15" customHeight="1">
+    <row r="18" spans="1:26" ht="45">
       <c r="A18" s="9" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D18" s="10">
         <v>45930</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>137</v>
+      <c r="I18" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="J18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L18" s="9" t="s">
+      <c r="M18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="N18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -29749,10 +29757,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>

</xml_diff>